<commit_message>
Update: automatisation du coloriage des cases
pour les modules, il suffit de changer la durée pour changer le coloriage des cases
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\misso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C119C4BF-DBB4-455F-BE44-87AEEEC8370D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCD6BD7-7138-4832-B23E-6F2CFF42A2DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Projet</t>
   </si>
   <si>
-    <t>Durée</t>
-  </si>
-  <si>
     <t>Début</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Administration</t>
+  </si>
+  <si>
+    <t>Durée(J)</t>
   </si>
 </sst>
 </file>
@@ -96,13 +96,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,8 +108,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,11 +126,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -169,30 +164,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -470,7 +500,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,90 +584,90 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
       <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
         <v>4</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" t="s">
-        <v>10</v>
-      </c>
       <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
         <v>4</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>6</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>7</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>8</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" t="s">
-        <v>10</v>
-      </c>
       <c r="Z2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" t="s">
         <v>4</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <f>D3-C3</f>
+        <f>D3-C3+1</f>
         <v>21</v>
       </c>
       <c r="C3" s="1">
@@ -645,34 +675,36 @@
         <v>45733</v>
       </c>
       <c r="D3" s="1">
-        <f>AA1</f>
-        <v>45754</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+        <f>Z1</f>
+        <v>45753</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -682,86 +714,353 @@
         <v>45733</v>
       </c>
       <c r="D4" s="1">
-        <f>C4+B4</f>
+        <f>C4+B4-1</f>
+        <v>45737</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45732</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45733</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45734</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45735</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45736</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45737</v>
+      </c>
+      <c r="K4" s="4">
         <v>45738</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="L4" s="4">
+        <v>45739</v>
+      </c>
+      <c r="M4" s="4">
+        <v>45740</v>
+      </c>
+      <c r="N4" s="4">
+        <v>45741</v>
+      </c>
+      <c r="O4" s="4">
+        <v>45742</v>
+      </c>
+      <c r="P4" s="4">
+        <v>45743</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>45744</v>
+      </c>
+      <c r="R4" s="4">
+        <v>45745</v>
+      </c>
+      <c r="S4" s="4">
+        <v>45746</v>
+      </c>
+      <c r="T4" s="4">
+        <v>45747</v>
+      </c>
+      <c r="U4" s="4">
+        <v>45748</v>
+      </c>
+      <c r="V4" s="4">
+        <v>45749</v>
+      </c>
+      <c r="W4" s="4">
+        <v>45750</v>
+      </c>
+      <c r="X4" s="4">
+        <v>45751</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>45752</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>45753</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>45754</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <f>D4</f>
+        <f>D4+1</f>
         <v>45738</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D7" si="0">C5+B5</f>
+        <f>C5+B5-1</f>
+        <v>45744</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45732</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45733</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45734</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45735</v>
+      </c>
+      <c r="I5" s="4">
+        <v>45736</v>
+      </c>
+      <c r="J5" s="4">
+        <v>45737</v>
+      </c>
+      <c r="K5" s="4">
+        <v>45738</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45739</v>
+      </c>
+      <c r="M5" s="4">
+        <v>45740</v>
+      </c>
+      <c r="N5" s="4">
+        <v>45741</v>
+      </c>
+      <c r="O5" s="4">
+        <v>45742</v>
+      </c>
+      <c r="P5" s="4">
+        <v>45743</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>45744</v>
+      </c>
+      <c r="R5" s="4">
         <v>45745</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="S5" s="4">
+        <v>45746</v>
+      </c>
+      <c r="T5" s="4">
+        <v>45747</v>
+      </c>
+      <c r="U5" s="4">
+        <v>45748</v>
+      </c>
+      <c r="V5" s="4">
+        <v>45749</v>
+      </c>
+      <c r="W5" s="4">
+        <v>45750</v>
+      </c>
+      <c r="X5" s="4">
+        <v>45751</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>45752</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>45753</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>45754</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C7" si="1">D5</f>
+        <f>D5+1</f>
         <v>45745</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D6:D7" si="0">C6+B6-1</f>
+        <v>45750</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45732</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45733</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45734</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45735</v>
+      </c>
+      <c r="I6" s="4">
+        <v>45736</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45737</v>
+      </c>
+      <c r="K6" s="4">
+        <v>45738</v>
+      </c>
+      <c r="L6" s="4">
+        <v>45739</v>
+      </c>
+      <c r="M6" s="4">
+        <v>45740</v>
+      </c>
+      <c r="N6" s="4">
+        <v>45741</v>
+      </c>
+      <c r="O6" s="4">
+        <v>45742</v>
+      </c>
+      <c r="P6" s="4">
+        <v>45743</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>45744</v>
+      </c>
+      <c r="R6" s="4">
+        <v>45745</v>
+      </c>
+      <c r="S6" s="4">
+        <v>45746</v>
+      </c>
+      <c r="T6" s="4">
+        <v>45747</v>
+      </c>
+      <c r="U6" s="4">
+        <v>45748</v>
+      </c>
+      <c r="V6" s="4">
+        <v>45749</v>
+      </c>
+      <c r="W6" s="4">
+        <v>45750</v>
+      </c>
+      <c r="X6" s="4">
         <v>45751</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
+      <c r="Y6" s="4">
+        <v>45752</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>45753</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>45754</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f>D6+1</f>
         <v>45751</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
+        <v>45753</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45732</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45733</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45734</v>
+      </c>
+      <c r="H7" s="4">
+        <v>45735</v>
+      </c>
+      <c r="I7" s="4">
+        <v>45736</v>
+      </c>
+      <c r="J7" s="4">
+        <v>45737</v>
+      </c>
+      <c r="K7" s="4">
+        <v>45738</v>
+      </c>
+      <c r="L7" s="4">
+        <v>45739</v>
+      </c>
+      <c r="M7" s="4">
+        <v>45740</v>
+      </c>
+      <c r="N7" s="4">
+        <v>45741</v>
+      </c>
+      <c r="O7" s="4">
+        <v>45742</v>
+      </c>
+      <c r="P7" s="4">
+        <v>45743</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>45744</v>
+      </c>
+      <c r="R7" s="4">
+        <v>45745</v>
+      </c>
+      <c r="S7" s="4">
+        <v>45746</v>
+      </c>
+      <c r="T7" s="4">
+        <v>45747</v>
+      </c>
+      <c r="U7" s="4">
+        <v>45748</v>
+      </c>
+      <c r="V7" s="4">
+        <v>45749</v>
+      </c>
+      <c r="W7" s="4">
+        <v>45750</v>
+      </c>
+      <c r="X7" s="4">
+        <v>45751</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>45752</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>45753</v>
+      </c>
+      <c r="AA7" s="4">
         <v>45754</v>
       </c>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="E8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="Y8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E4:AA7">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>$C4</formula>
+      <formula>$D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:AA4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>$C4</formula>
+      <formula>$D4-1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update: dates des rdv
dans planification: case jaune = rdv
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\misso\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DB69EB-E72A-4337-9736-CFE7357147BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,85 +27,65 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
-    <t xml:space="preserve">Projet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durée(J)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Début</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dimanche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lundi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mardi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercredi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeudi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendredi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samedi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Misso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administration</t>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Durée(J)</t>
+  </si>
+  <si>
+    <t>Début</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Dimanche</t>
+  </si>
+  <si>
+    <t>Lundi</t>
+  </si>
+  <si>
+    <t>Mardi</t>
+  </si>
+  <si>
+    <t>Mercredi</t>
+  </si>
+  <si>
+    <t>Jeudi</t>
+  </si>
+  <si>
+    <t>Vendredi</t>
+  </si>
+  <si>
+    <t>Samedi</t>
+  </si>
+  <si>
+    <t>Misso</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Visualisation</t>
+  </si>
+  <si>
+    <t>Gestion</t>
+  </si>
+  <si>
+    <t>Administration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -158,14 +143,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFB1BBCC"/>
       </left>
@@ -181,76 +166,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="3">
+    <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Good" xfId="20"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="21"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -274,6 +209,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -332,60 +268,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -417,7 +369,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -441,7 +393,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -501,198 +453,197 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.44"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E1" s="1" t="n">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="E1" s="1">
         <v>45732</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="1">
         <v>45733</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="1">
         <v>45734</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="1">
         <v>45735</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="1">
         <v>45736</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="1">
         <v>45737</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="1">
         <v>45738</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="1">
         <v>45739</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="1">
         <v>45740</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="1">
         <v>45741</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="1">
         <v>45742</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="1">
         <v>45743</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="1">
         <v>45744</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="1">
         <v>45745</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="1">
         <v>45746</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="1">
         <v>45747</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="1">
         <v>45748</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="1">
         <v>45749</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="1">
         <v>45750</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="1">
         <v>45751</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="1">
         <v>45752</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="1">
         <v>45753</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="1">
         <v>45754</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <f aca="false">D3-C3+1</f>
+      <c r="B3" s="3">
+        <f>D3-C3+1</f>
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <f aca="false">F1</f>
+      <c r="C3" s="1">
+        <f>F1</f>
         <v>45733</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">Z1</f>
+      <c r="D3" s="1">
+        <f>Z1</f>
         <v>45753</v>
       </c>
       <c r="E3" s="1"/>
@@ -719,371 +670,366 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <f aca="false">C3</f>
+      <c r="C4" s="1">
+        <f>C3</f>
         <v>45733</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">C4+B4-1</f>
+      <c r="D4" s="1">
+        <f>C4+B4-1</f>
         <v>45740</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="5">
         <v>45732</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="5">
         <v>45733</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="5">
         <v>45734</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="5">
         <v>45735</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="5">
         <v>45736</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="5">
         <v>45737</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="5">
         <v>45738</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="5">
         <v>45739</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="5">
         <v>45740</v>
       </c>
-      <c r="N4" s="5" t="n">
+      <c r="N4" s="5">
         <v>45741</v>
       </c>
-      <c r="O4" s="5" t="n">
+      <c r="O4" s="5">
         <v>45742</v>
       </c>
-      <c r="P4" s="5" t="n">
+      <c r="P4" s="5">
         <v>45743</v>
       </c>
-      <c r="Q4" s="5" t="n">
+      <c r="Q4" s="5">
         <v>45744</v>
       </c>
-      <c r="R4" s="5" t="n">
+      <c r="R4" s="5">
         <v>45745</v>
       </c>
-      <c r="S4" s="5" t="n">
+      <c r="S4" s="5">
         <v>45746</v>
       </c>
-      <c r="T4" s="5" t="n">
+      <c r="T4" s="5">
         <v>45747</v>
       </c>
-      <c r="U4" s="5" t="n">
+      <c r="U4" s="5">
         <v>45748</v>
       </c>
-      <c r="V4" s="5" t="n">
+      <c r="V4" s="5">
         <v>45749</v>
       </c>
-      <c r="W4" s="5" t="n">
+      <c r="W4" s="5">
         <v>45750</v>
       </c>
-      <c r="X4" s="5" t="n">
+      <c r="X4" s="5">
         <v>45751</v>
       </c>
-      <c r="Y4" s="5" t="n">
+      <c r="Y4" s="5">
         <v>45752</v>
       </c>
-      <c r="Z4" s="5" t="n">
+      <c r="Z4" s="5">
         <v>45753</v>
       </c>
-      <c r="AA4" s="5" t="n">
+      <c r="AA4" s="5">
         <v>45754</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <f aca="false">D4+1</f>
+      <c r="C5" s="1">
+        <f>D4+1</f>
         <v>45741</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">C5+B5-1</f>
+      <c r="D5" s="1">
+        <f>C5+B5-1</f>
         <v>45748</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="5">
         <v>45732</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="5">
         <v>45733</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="5">
         <v>45734</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>45735</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="5">
         <v>45736</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="5">
         <v>45737</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="5">
         <v>45738</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="5">
         <v>45739</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="5">
         <v>45740</v>
       </c>
-      <c r="N5" s="5" t="n">
+      <c r="N5" s="5">
         <v>45741</v>
       </c>
-      <c r="O5" s="5" t="n">
+      <c r="O5" s="5">
         <v>45742</v>
       </c>
-      <c r="P5" s="5" t="n">
+      <c r="P5" s="5">
         <v>45743</v>
       </c>
-      <c r="Q5" s="5" t="n">
+      <c r="Q5" s="5">
         <v>45744</v>
       </c>
-      <c r="R5" s="5" t="n">
+      <c r="R5" s="5">
         <v>45745</v>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S5" s="5">
         <v>45746</v>
       </c>
-      <c r="T5" s="5" t="n">
+      <c r="T5" s="5">
         <v>45747</v>
       </c>
-      <c r="U5" s="5" t="n">
+      <c r="U5" s="5">
         <v>45748</v>
       </c>
-      <c r="V5" s="5" t="n">
+      <c r="V5" s="5">
         <v>45749</v>
       </c>
-      <c r="W5" s="5" t="n">
+      <c r="W5" s="5">
         <v>45750</v>
       </c>
-      <c r="X5" s="5" t="n">
+      <c r="X5" s="5">
         <v>45751</v>
       </c>
-      <c r="Y5" s="5" t="n">
+      <c r="Y5" s="5">
         <v>45752</v>
       </c>
-      <c r="Z5" s="5" t="n">
+      <c r="Z5" s="5">
         <v>45753</v>
       </c>
-      <c r="AA5" s="5" t="n">
+      <c r="AA5" s="5">
         <v>45754</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <f aca="false">D5+1</f>
+      <c r="C6" s="1">
+        <f>D5+1</f>
         <v>45749</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">C6+B6-1</f>
+      <c r="D6" s="1">
+        <f>C6+B6-1</f>
         <v>45750</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="5">
         <v>45732</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="5">
         <v>45733</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="5">
         <v>45734</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="5">
         <v>45735</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="5">
         <v>45736</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="5">
         <v>45737</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="5">
         <v>45738</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="5">
         <v>45739</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="5">
         <v>45740</v>
       </c>
-      <c r="N6" s="5" t="n">
+      <c r="N6" s="5">
         <v>45741</v>
       </c>
-      <c r="O6" s="5" t="n">
+      <c r="O6" s="5">
         <v>45742</v>
       </c>
-      <c r="P6" s="5" t="n">
+      <c r="P6" s="5">
         <v>45743</v>
       </c>
-      <c r="Q6" s="5" t="n">
+      <c r="Q6" s="5">
         <v>45744</v>
       </c>
-      <c r="R6" s="5" t="n">
+      <c r="R6" s="5">
         <v>45745</v>
       </c>
-      <c r="S6" s="5" t="n">
+      <c r="S6" s="5">
         <v>45746</v>
       </c>
-      <c r="T6" s="5" t="n">
+      <c r="T6" s="5">
         <v>45747</v>
       </c>
-      <c r="U6" s="5" t="n">
+      <c r="U6" s="5">
         <v>45748</v>
       </c>
-      <c r="V6" s="5" t="n">
+      <c r="V6" s="5">
         <v>45749</v>
       </c>
-      <c r="W6" s="5" t="n">
+      <c r="W6" s="5">
         <v>45750</v>
       </c>
-      <c r="X6" s="5" t="n">
+      <c r="X6" s="5">
         <v>45751</v>
       </c>
-      <c r="Y6" s="5" t="n">
+      <c r="Y6" s="5">
         <v>45752</v>
       </c>
-      <c r="Z6" s="5" t="n">
+      <c r="Z6" s="5">
         <v>45753</v>
       </c>
-      <c r="AA6" s="5" t="n">
+      <c r="AA6" s="5">
         <v>45754</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <f aca="false">D6+1</f>
+      <c r="C7" s="1">
+        <f>D6+1</f>
         <v>45751</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">C7+B7-1</f>
+      <c r="D7" s="1">
+        <f>C7+B7-1</f>
         <v>45752</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="5">
         <v>45732</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="5">
         <v>45733</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="5">
         <v>45734</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="5">
         <v>45735</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="5">
         <v>45736</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="5">
         <v>45737</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="5">
         <v>45738</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="5">
         <v>45739</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="5">
         <v>45740</v>
       </c>
-      <c r="N7" s="5" t="n">
+      <c r="N7" s="5">
         <v>45741</v>
       </c>
-      <c r="O7" s="5" t="n">
+      <c r="O7" s="5">
         <v>45742</v>
       </c>
-      <c r="P7" s="5" t="n">
+      <c r="P7" s="5">
         <v>45743</v>
       </c>
-      <c r="Q7" s="5" t="n">
+      <c r="Q7" s="5">
         <v>45744</v>
       </c>
-      <c r="R7" s="5" t="n">
+      <c r="R7" s="5">
         <v>45745</v>
       </c>
-      <c r="S7" s="5" t="n">
+      <c r="S7" s="5">
         <v>45746</v>
       </c>
-      <c r="T7" s="5" t="n">
+      <c r="T7" s="5">
         <v>45747</v>
       </c>
-      <c r="U7" s="5" t="n">
+      <c r="U7" s="5">
         <v>45748</v>
       </c>
-      <c r="V7" s="5" t="n">
+      <c r="V7" s="5">
         <v>45749</v>
       </c>
-      <c r="W7" s="5" t="n">
+      <c r="W7" s="5">
         <v>45750</v>
       </c>
-      <c r="X7" s="5" t="n">
+      <c r="X7" s="5">
         <v>45751</v>
       </c>
-      <c r="Y7" s="5" t="n">
+      <c r="Y7" s="5">
         <v>45752</v>
       </c>
-      <c r="Z7" s="5" t="n">
+      <c r="Z7" s="5">
         <v>45753</v>
       </c>
-      <c r="AA7" s="5" t="n">
+      <c r="AA7" s="5">
         <v>45754</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="Z8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="U8" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:AA4">
-    <cfRule type="cellIs" priority="2" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>$C4</formula>
       <formula>$D4-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AA7">
-    <cfRule type="cellIs" priority="3" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>$C4</formula>
       <formula>$D4</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>